<commit_message>
PIN-2681: Usage of Enum constraint
</commit_message>
<xml_diff>
--- a/tests/NewApiBundle/Resources/SYR-only-camp-1HH.xlsx
+++ b/tests/NewApiBundle/Resources/SYR-only-camp-1HH.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="133">
   <si>
     <t xml:space="preserve">Address street</t>
   </si>
@@ -420,9 +420,6 @@
   </si>
   <si>
     <t xml:space="preserve">23-03-1982</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID Card</t>
   </si>
 </sst>
 </file>
@@ -530,30 +527,31 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BE6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AO13" activeCellId="0" sqref="AO13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="12.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1204,7 +1202,7 @@
         <v>132</v>
       </c>
       <c r="AK6" s="0" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="AL6" s="0" t="n">
         <v>9999</v>
@@ -1243,7 +1241,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1252,7 +1250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1262,14 +1260,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>